<commit_message>
add timecost xlsx figure
</commit_message>
<xml_diff>
--- a/vConvFigmain/files.AdditionalTImecost/timecost.xlsx
+++ b/vConvFigmain/files.AdditionalTImecost/timecost.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DDE99-9100-4B84-BE02-05562F547C83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1(with figure)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>Data name</t>
   </si>
@@ -95,12 +97,15 @@
   </si>
   <si>
     <t>0.704s</t>
+  </si>
+  <si>
+    <t>Convolution-based network</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -207,6 +212,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -226,8 +234,1252 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vConv-based network</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$F$3:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2 motifs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 motifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6 motifs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 motifs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TwoDiffMotif1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TwoDiffMotif2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TwoDiffMotif3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1(with figure)'!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70399999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA56-4D05-B7BA-A018FF619074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Convolution-based network</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$F$3:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2 motifs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 motifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6 motifs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 motifs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TwoDiffMotif1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TwoDiffMotif2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TwoDiffMotif3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1(with figure)'!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59899999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BA56-4D05-B7BA-A018FF619074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="138249343"/>
+        <c:axId val="138244351"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vConv-based network</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$F$3:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2 motifs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 motifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6 motifs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 motifs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TwoDiffMotif1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TwoDiffMotif2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TwoDiffMotif3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1(with figure)'!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BA56-4D05-B7BA-A018FF619074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Convolution-based network</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1(with figure)'!$F$3:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2 motifs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 motifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6 motifs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 motifs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TwoDiffMotif1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TwoDiffMotif2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TwoDiffMotif3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1(with figure)'!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BA56-4D05-B7BA-A018FF619074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="138194847"/>
+        <c:axId val="138202751"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="138249343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="138244351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="138244351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="138249343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="138202751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="138194847"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="138194847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="138202751"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>226218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>588168</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>64293</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7CB01E0-D6EB-4CDE-8159-8BBC557FF6F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -302,6 +1554,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -337,6 +1606,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -512,21 +1798,387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F32FB6-A2D2-4228-B6CB-51C7333454BE}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.623</v>
+      </c>
+      <c r="D3" s="4">
+        <v>82</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.623</v>
+      </c>
+      <c r="I3" s="4">
+        <v>100</v>
+      </c>
+      <c r="J3" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="I4" s="4">
+        <v>93</v>
+      </c>
+      <c r="J4" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I5" s="4">
+        <v>80</v>
+      </c>
+      <c r="J5" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="D6" s="4">
+        <v>93</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="I6" s="4">
+        <v>84</v>
+      </c>
+      <c r="J6" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="D7" s="4">
+        <v>89</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="I7" s="4">
+        <v>100</v>
+      </c>
+      <c r="J7" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D8" s="4">
+        <v>80</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>101</v>
+      </c>
+      <c r="J8" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="D9" s="4">
+        <v>65</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="I9" s="4">
+        <v>97</v>
+      </c>
+      <c r="J9" s="4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="D10" s="4">
+        <v>84</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="D11" s="4">
+        <v>94</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="D12" s="4">
+        <v>100</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="D13" s="4">
+        <v>94</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="D14" s="4">
+        <v>101</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="D15" s="4">
+        <v>101</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="D16" s="4">
+        <v>97</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +2192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -554,7 +2206,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -568,7 +2220,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -582,7 +2234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -596,7 +2248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -610,7 +2262,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -624,7 +2276,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -638,7 +2290,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -652,7 +2304,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -666,7 +2318,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -680,7 +2332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -694,7 +2346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -708,7 +2360,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -722,7 +2374,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>